<commit_message>
report on old finish + predictions on new
</commit_message>
<xml_diff>
--- a/reports/Airline dataset - report 1.xlsx
+++ b/reports/Airline dataset - report 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\OneDrive\Desktop\Portfolio\Flight-Price-EDA\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9890B48-1E28-4291-ADCE-03DCF51860D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36917B46-C8A1-46BB-9FF1-DE13E7DCC18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Linear Regression</t>
   </si>
@@ -37,6 +37,69 @@
 Mean squared error : 10291432.749936875
 Mean absoute error : 2081.05700941328
 RMSE3208.0263013162585</t>
+  </si>
+  <si>
+    <t>SVM Regressor</t>
+  </si>
+  <si>
+    <t>R2 score : -384959382.9359258
+MSE : 22492360.669205155
+MAE : 3648.9522817089223
+RMSE : 4742.611165719277</t>
+  </si>
+  <si>
+    <t>KNN(without tunning)</t>
+  </si>
+  <si>
+    <t>R2 score : 0.3024309610279875
+MSE : 9296390.005915388
+MAE : 1855.2743541744667
+RMSE : 3048.9981970993995</t>
+  </si>
+  <si>
+    <t>KNN(With tunning)</t>
+  </si>
+  <si>
+    <t>R2 score : 0.361634207484813
+MSE : 8880710.311628217
+MAE : 1791.5204470886295
+RMSE : 2980.0520652546015</t>
+  </si>
+  <si>
+    <t>Random forest regressor</t>
+  </si>
+  <si>
+    <t>R2 score : 0.8407217255724877
+MSE : 3037696.667942037
+MAE : 706.5036291041938
+RMSE : 1742.8989264848483</t>
+  </si>
+  <si>
+    <t>Decision Tree regressor</t>
+  </si>
+  <si>
+    <t>R2 score : 0.7898977600332686
+MSE : 4334240.916531471
+MAE : 809.7973293398229
+RMSE : 2081.8839824859288</t>
+  </si>
+  <si>
+    <t>Adaboost regression</t>
+  </si>
+  <si>
+    <t>R2 score : -0.25187375100265186
+MSE : 14842884.794488242
+MAE : 3011.8329710157254
+RMSE : 3852.646466325225</t>
+  </si>
+  <si>
+    <t>Gradient BOOST</t>
+  </si>
+  <si>
+    <t>R2 score : 0.6592823156099847
+MSE : 5083627.683108177
+MAE : 1345.8371341566426
+RMSE : 2254.690152350912</t>
   </si>
 </sst>
 </file>
@@ -104,12 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -117,6 +180,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -173,6 +248,314 @@
         <a:xfrm>
           <a:off x="15240" y="2072641"/>
           <a:ext cx="5021580" cy="3276600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>7621</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56831E0F-A8C0-C2C2-B13E-00AA13E41775}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="2057401"/>
+          <a:ext cx="4899660" cy="3299460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>48846</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D0548EB-E9A1-BA0F-151D-A776C681AE9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10902462" y="2080846"/>
+          <a:ext cx="4894384" cy="3341077"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>87924</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>146539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CFA998D-C4D8-C0E3-3D62-176636679294}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7278078"/>
+          <a:ext cx="4933462" cy="3302000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>68385</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2620683-7EF2-FB52-2368-846770BE1FA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5451231" y="7278078"/>
+          <a:ext cx="4913923" cy="3272692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>78154</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>39077</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF06591-0565-0F2B-6BCE-1F279F8968D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10902462" y="7493001"/>
+          <a:ext cx="4923692" cy="3194538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68385</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>29309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58694F1D-1A7E-2D2C-A8E9-10B12F0B6657}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12690232"/>
+          <a:ext cx="4913923" cy="3556000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>68385</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>9769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D410D45-29D2-5CC8-DB3F-14DF5A49361B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5451231" y="12690231"/>
+          <a:ext cx="4913923" cy="3536461"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -447,86 +830,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -537,8 +920,28 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="S4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -547,8 +950,24 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -559,8 +978,28 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="S6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -569,8 +1008,24 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -579,8 +1034,24 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -589,8 +1060,24 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -599,8 +1086,24 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -609,8 +1112,24 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -620,11 +1139,397 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
+    <row r="32" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="J32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="S32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+    </row>
+    <row r="33" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="J34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="S34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+    </row>
+    <row r="39" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="J60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="J62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="17">
+    <mergeCell ref="A60:H61"/>
+    <mergeCell ref="A62:H67"/>
+    <mergeCell ref="J60:Q61"/>
+    <mergeCell ref="J62:Q67"/>
+    <mergeCell ref="A32:H33"/>
+    <mergeCell ref="A34:H39"/>
+    <mergeCell ref="J32:Q33"/>
+    <mergeCell ref="J34:Q39"/>
+    <mergeCell ref="S32:Z33"/>
+    <mergeCell ref="S34:Z39"/>
     <mergeCell ref="A1:U3"/>
     <mergeCell ref="A4:H5"/>
     <mergeCell ref="A6:H12"/>
+    <mergeCell ref="J4:Q5"/>
+    <mergeCell ref="J6:Q11"/>
+    <mergeCell ref="S4:Z5"/>
+    <mergeCell ref="S6:Z11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>